<commit_message>
Scoring version 0.2 - complete. Fixed all bugs with sources/parsers Fix bug with order of sources (now all order is according to scoring) IMPORTANT NOTE - USE SOURCES ONLY FROM REPO Added requirements file. Added shorten logs in ops history. Fix NBKI parser. Added logging files for processors with STDOUT redirect.
</commit_message>
<xml_diff>
--- a/core/test_data/test_users.xlsx
+++ b/core/test_data/test_users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justkru/Documents/GitHub/willz-dev/core/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA40A623-CE10-ED4C-8B58-730E02EFB9D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A371D92C-A760-6B44-BB38-66FA26382F37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="28940" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16297,10 +16297,10 @@
     <t>Москва, Ленина, 1-1</t>
   </si>
   <si>
-    <t>4518 333452</t>
-  </si>
-  <si>
     <t>77 МА 051161</t>
+  </si>
+  <si>
+    <t>4518 334452</t>
   </si>
 </sst>
 </file>
@@ -16712,8 +16712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH305"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17009,7 +17009,7 @@
         <v>56</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>5425</v>
+        <v>5426</v>
       </c>
       <c r="AH2" s="5" t="s">
         <v>5422</v>
@@ -17081,7 +17081,7 @@
         <v>63</v>
       </c>
       <c r="BF2" s="7" t="s">
-        <v>5426</v>
+        <v>5425</v>
       </c>
       <c r="BG2" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
update of test data
</commit_message>
<xml_diff>
--- a/core/test_data/test_users.xlsx
+++ b/core/test_data/test_users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justkru/Documents/GitHub/willz-dev/core/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD0CAA6-3361-8848-B0B0-9135C186CA2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F392E25C-BE71-5E4D-8F09-23B01E4EFADA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="28940" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16803,8 +16803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH305"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="AL25" sqref="AL25"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BA2" sqref="BA2:BD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17079,25 +17079,25 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>2056</v>
+        <v>206</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="s">
-        <v>2057</v>
+        <v>207</v>
       </c>
       <c r="AC2">
         <v>1</v>
       </c>
       <c r="AD2" t="s">
-        <v>2058</v>
+        <v>208</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF2" t="s">
-        <v>56</v>
+        <v>208</v>
       </c>
       <c r="AG2" s="5" t="s">
         <v>5424</v>
@@ -17163,13 +17163,13 @@
         <v>1</v>
       </c>
       <c r="BB2" t="s">
-        <v>62</v>
+        <v>213</v>
       </c>
       <c r="BC2">
         <v>1</v>
       </c>
       <c r="BD2" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="BF2" s="7" t="s">
         <v>5423</v>

</xml_diff>